<commit_message>
feat: add employee name export
</commit_message>
<xml_diff>
--- a/public/templates/car_template.xlsx
+++ b/public/templates/car_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\esetda-parkir\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F831D21A-B90D-4F4F-A137-5659288DED70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88D772A-D6FE-4F26-B5DA-AAD93853D0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0640265E-8207-4782-96EC-62AF41E75A86}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>No.</t>
   </si>
@@ -55,6 +46,9 @@
   </si>
   <si>
     <t>Tipe</t>
+  </si>
+  <si>
+    <t>Nama Pegawai</t>
   </si>
 </sst>
 </file>
@@ -444,19 +438,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741CA7BA-BED0-4D1B-946B-1C70C3D2A041}">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,38 +459,44 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>